<commit_message>
filled out peer review form
</commit_message>
<xml_diff>
--- a/.github/peer_review_issue (2).xlsx
+++ b/.github/peer_review_issue (2).xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11122"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elieliason/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F1B6831-316C-DA45-B971-0524402C836E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33296EB3-76E3-6F4F-A494-B2D05E984C25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1360" yWindow="680" windowWidth="28040" windowHeight="17200" xr2:uid="{D66B348C-C68D-BB42-8C69-2652486EB8F3}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Group No:</t>
   </si>
@@ -66,13 +66,31 @@
   </si>
   <si>
     <t>Neil Gopalan</t>
+  </si>
+  <si>
+    <t>Arshan Bari Rafiq</t>
+  </si>
+  <si>
+    <t>Jonathan Takuya Irwanto </t>
+  </si>
+  <si>
+    <t>One thing you could maybe add next time is a short explanation of why the indicators might have had no predictive power, just to give more context.”</t>
+  </si>
+  <si>
+    <t>Based on the presentation you showed in class, one thing I liked about it is that you used many predictor variables in your statistics. You used R&amp;D, profit, market cap, revenue, EPS, and operating expenses. Also, you plotted those predictor variables on the coefficient plot, and I thought it was interesting that there was no significant correlation.</t>
+  </si>
+  <si>
+    <t>thank you!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The indicators have no predictive value because the our tests showed supportive p-values and R squared values for our conclusions, we highlighted this during out presenation. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -82,6 +100,18 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF273540"/>
       <name val="Aptos Narrow"/>
       <scheme val="minor"/>
     </font>
@@ -106,12 +136,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,90 +496,118 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="29.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" customWidth="1"/>
+    <col min="3" max="3" width="71.6640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="62.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1"/>
-      <c r="D1"/>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
     </row>
     <row r="2" spans="1:4">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="3">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" s="3"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="B3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3">
         <v>2</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="D3"/>
+      <c r="D3" s="3"/>
     </row>
     <row r="4" spans="1:4">
-      <c r="B4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3">
         <v>3</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D4"/>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="B5">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D5"/>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
-      <c r="A7">
+    <row r="7" spans="1:4" ht="66" customHeight="1">
+      <c r="A7" s="3">
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8">
+      <c r="B7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="51">
+      <c r="A8" s="3">
         <v>2</v>
       </c>
+      <c r="B8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9">
+      <c r="A9" s="3">
         <v>3</v>
       </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="4"/>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10">
+      <c r="A10" s="3">
         <v>4</v>
       </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>